<commit_message>
Update the Dataset S2 after updating the input table
</commit_message>
<xml_diff>
--- a/06-figures_tables/Dataset_S2.xlsx
+++ b/06-figures_tables/Dataset_S2.xlsx
@@ -1918,10 +1918,10 @@
         <v>3276</v>
       </c>
       <c r="D21" s="2">
-        <v>0</v>
+        <v>1167</v>
       </c>
       <c r="E21" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F21" s="2">
         <v>0</v>
@@ -3478,16 +3478,16 @@
         <v>14946</v>
       </c>
       <c r="D45" s="2">
-        <v>0</v>
+        <v>4885</v>
       </c>
       <c r="E45" s="2">
-        <v>0</v>
+        <v>319</v>
       </c>
       <c r="F45" s="2">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="G45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Add pyDamage results to Dataset S2
</commit_message>
<xml_diff>
--- a/06-figures_tables/Dataset_S2.xlsx
+++ b/06-figures_tables/Dataset_S2.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="S2a - de novo assembly stats" sheetId="1" r:id="rId1"/>
     <sheet name="S2b - consensus correction" sheetId="2" r:id="rId2"/>
+    <sheet name="S2c - pyDamage analysis" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="128">
   <si>
     <t>BAN001</t>
   </si>
@@ -254,12 +255,6 @@
     <t>N100</t>
   </si>
   <si>
-    <t>CDS</t>
-  </si>
-  <si>
-    <t>genes</t>
-  </si>
-  <si>
     <t>SPM001</t>
   </si>
   <si>
@@ -342,15 +337,80 @@
   </si>
   <si>
     <t>90% &lt; AF &lt;= 100%</t>
+  </si>
+  <si>
+    <t>Table S2c: Overview of the evaluation of the presence of ancient DNA damage using pyDamage. We only considered contigs that had a minimal coverage of 5-fold to avoid wrong inference due to the lack of sufficient data. From these contigs, we considered the contigs 'ancient', when the q-value returned by pyDamage was &lt; 0.05. The columns '15% &lt;= PA &lt; 20%' to '95% &lt;= PA &lt; 100%' summarise the number of contigs that had a predicted accuracy (PA) in this range.</t>
+  </si>
+  <si>
+    <t>total # of contigs</t>
+  </si>
+  <si>
+    <t>% of contigs with coverage &gt;= 5x</t>
+  </si>
+  <si>
+    <t>% of contigs with q-value &lt; 0.05</t>
+  </si>
+  <si>
+    <t>15% &lt;= PA &lt; 20%</t>
+  </si>
+  <si>
+    <t>20% &lt;= PA &lt; 25%</t>
+  </si>
+  <si>
+    <t>25% &lt;= PA &lt; 30%</t>
+  </si>
+  <si>
+    <t>30% &lt;= PA &lt; 35%</t>
+  </si>
+  <si>
+    <t>35% &lt;= PA &lt; 40%</t>
+  </si>
+  <si>
+    <t>40% &lt;= PA &lt; 45%</t>
+  </si>
+  <si>
+    <t>45% &lt;= PA &lt; 50%</t>
+  </si>
+  <si>
+    <t>50% &lt;= PA &lt; 55%</t>
+  </si>
+  <si>
+    <t>55% &lt;= PA &lt; 60%</t>
+  </si>
+  <si>
+    <t>60% &lt;= PA &lt; 65%</t>
+  </si>
+  <si>
+    <t>65% &lt;= PA &lt; 70%</t>
+  </si>
+  <si>
+    <t>70% &lt;= PA &lt; 75%</t>
+  </si>
+  <si>
+    <t>75% &lt;= PA &lt; 80%</t>
+  </si>
+  <si>
+    <t>80% &lt;= PA &lt; 85%</t>
+  </si>
+  <si>
+    <t>85% &lt;= PA &lt; 90%</t>
+  </si>
+  <si>
+    <t>90% &lt;= PA &lt; 95%</t>
+  </si>
+  <si>
+    <t>95% &lt;= PA &lt; 100%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -389,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -407,6 +467,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -703,20 +769,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U62"/>
+  <dimension ref="A1:S62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="27.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="8.7109375" style="2" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" style="2" customWidth="1"/>
@@ -728,16 +794,14 @@
     <col min="17" max="17" width="6.7109375" style="2" customWidth="1"/>
     <col min="18" max="18" width="6.7109375" style="2" customWidth="1"/>
     <col min="19" max="19" width="6.7109375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="8.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:19">
       <c r="A1" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:19">
       <c r="A3" s="4" t="s">
         <v>60</v>
       </c>
@@ -795,14 +859,8 @@
       <c r="S3" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="T3" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -860,14 +918,8 @@
       <c r="S4" s="2">
         <v>500</v>
       </c>
-      <c r="T4" s="2">
-        <v>25423</v>
-      </c>
-      <c r="U4" s="2">
-        <v>25494</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -925,14 +977,8 @@
       <c r="S5" s="2">
         <v>500</v>
       </c>
-      <c r="T5" s="2">
-        <v>25220</v>
-      </c>
-      <c r="U5" s="2">
-        <v>25294</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -990,14 +1036,8 @@
       <c r="S6" s="2">
         <v>500</v>
       </c>
-      <c r="T6" s="2">
-        <v>39285</v>
-      </c>
-      <c r="U6" s="2">
-        <v>39720</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1055,14 +1095,8 @@
       <c r="S7" s="2">
         <v>500</v>
       </c>
-      <c r="T7" s="2">
-        <v>53399</v>
-      </c>
-      <c r="U7" s="2">
-        <v>53762</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1120,14 +1154,8 @@
       <c r="S8" s="2">
         <v>500</v>
       </c>
-      <c r="T8" s="2">
-        <v>275</v>
-      </c>
-      <c r="U8" s="2">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1185,14 +1213,8 @@
       <c r="S9" s="2">
         <v>500</v>
       </c>
-      <c r="T9" s="2">
-        <v>17364</v>
-      </c>
-      <c r="U9" s="2">
-        <v>17637</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1250,14 +1272,8 @@
       <c r="S10" s="2">
         <v>500</v>
       </c>
-      <c r="T10" s="2">
-        <v>105745</v>
-      </c>
-      <c r="U10" s="2">
-        <v>106990</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1315,14 +1331,8 @@
       <c r="S11" s="2">
         <v>500</v>
       </c>
-      <c r="T11" s="2">
-        <v>5545</v>
-      </c>
-      <c r="U11" s="2">
-        <v>5602</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1380,14 +1390,8 @@
       <c r="S12" s="2">
         <v>500</v>
       </c>
-      <c r="T12" s="2">
-        <v>2254</v>
-      </c>
-      <c r="U12" s="2">
-        <v>2305</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1445,14 +1449,8 @@
       <c r="S13" s="2">
         <v>500</v>
       </c>
-      <c r="T13" s="2">
-        <v>12575</v>
-      </c>
-      <c r="U13" s="2">
-        <v>12783</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1510,14 +1508,8 @@
       <c r="S14" s="2">
         <v>500</v>
       </c>
-      <c r="T14" s="2">
-        <v>9303</v>
-      </c>
-      <c r="U14" s="2">
-        <v>9459</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1575,14 +1567,8 @@
       <c r="S15" s="2">
         <v>500</v>
       </c>
-      <c r="T15" s="2">
-        <v>10747</v>
-      </c>
-      <c r="U15" s="2">
-        <v>10891</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1640,14 +1626,8 @@
       <c r="S16" s="2">
         <v>500</v>
       </c>
-      <c r="T16" s="2">
-        <v>796</v>
-      </c>
-      <c r="U16" s="2">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21">
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1705,14 +1685,8 @@
       <c r="S17" s="2">
         <v>500</v>
       </c>
-      <c r="T17" s="2">
-        <v>35421</v>
-      </c>
-      <c r="U17" s="2">
-        <v>35772</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -1770,14 +1744,8 @@
       <c r="S18" s="2">
         <v>500</v>
       </c>
-      <c r="T18" s="2">
-        <v>15168</v>
-      </c>
-      <c r="U18" s="2">
-        <v>15354</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -1835,14 +1803,8 @@
       <c r="S19" s="2">
         <v>500</v>
       </c>
-      <c r="T19" s="2">
-        <v>122795</v>
-      </c>
-      <c r="U19" s="2">
-        <v>123327</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -1900,14 +1862,8 @@
       <c r="S20" s="2">
         <v>500</v>
       </c>
-      <c r="T20" s="2">
-        <v>17014</v>
-      </c>
-      <c r="U20" s="2">
-        <v>17239</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -1965,14 +1921,8 @@
       <c r="S21" s="2">
         <v>500</v>
       </c>
-      <c r="T21" s="2">
-        <v>3475</v>
-      </c>
-      <c r="U21" s="2">
-        <v>3527</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21">
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -2030,14 +1980,8 @@
       <c r="S22" s="2">
         <v>500</v>
       </c>
-      <c r="T22" s="2">
-        <v>80472</v>
-      </c>
-      <c r="U22" s="2">
-        <v>81589</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21">
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -2095,14 +2039,8 @@
       <c r="S23" s="2">
         <v>500</v>
       </c>
-      <c r="T23" s="2">
-        <v>67761</v>
-      </c>
-      <c r="U23" s="2">
-        <v>68712</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21">
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -2160,14 +2098,8 @@
       <c r="S24" s="2">
         <v>500</v>
       </c>
-      <c r="T24" s="2">
-        <v>138575</v>
-      </c>
-      <c r="U24" s="2">
-        <v>140296</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -2225,14 +2157,8 @@
       <c r="S25" s="2">
         <v>500</v>
       </c>
-      <c r="T25" s="2">
-        <v>131379</v>
-      </c>
-      <c r="U25" s="2">
-        <v>133148</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21">
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -2290,14 +2216,8 @@
       <c r="S26" s="2">
         <v>500</v>
       </c>
-      <c r="T26" s="2">
-        <v>101274</v>
-      </c>
-      <c r="U26" s="2">
-        <v>102530</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21">
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -2355,14 +2275,8 @@
       <c r="S27" s="2">
         <v>500</v>
       </c>
-      <c r="T27" s="2">
-        <v>101921</v>
-      </c>
-      <c r="U27" s="2">
-        <v>103296</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21">
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -2420,14 +2334,8 @@
       <c r="S28" s="2">
         <v>500</v>
       </c>
-      <c r="T28" s="2">
-        <v>77328</v>
-      </c>
-      <c r="U28" s="2">
-        <v>78291</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -2485,14 +2393,8 @@
       <c r="S29" s="2">
         <v>500</v>
       </c>
-      <c r="T29" s="2">
-        <v>142867</v>
-      </c>
-      <c r="U29" s="2">
-        <v>144855</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21">
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
@@ -2550,14 +2452,8 @@
       <c r="S30" s="2">
         <v>500</v>
       </c>
-      <c r="T30" s="2">
-        <v>114314</v>
-      </c>
-      <c r="U30" s="2">
-        <v>115931</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21">
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -2615,14 +2511,8 @@
       <c r="S31" s="2">
         <v>500</v>
       </c>
-      <c r="T31" s="2">
-        <v>136407</v>
-      </c>
-      <c r="U31" s="2">
-        <v>138542</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21">
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
@@ -2680,14 +2570,8 @@
       <c r="S32" s="2">
         <v>500</v>
       </c>
-      <c r="T32" s="2">
-        <v>16259</v>
-      </c>
-      <c r="U32" s="2">
-        <v>16444</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21">
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
@@ -2745,14 +2629,8 @@
       <c r="S33" s="2">
         <v>500</v>
       </c>
-      <c r="T33" s="2">
-        <v>8203</v>
-      </c>
-      <c r="U33" s="2">
-        <v>8315</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21">
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34" s="1" t="s">
         <v>30</v>
       </c>
@@ -2810,14 +2688,8 @@
       <c r="S34" s="2">
         <v>500</v>
       </c>
-      <c r="T34" s="2">
-        <v>6641</v>
-      </c>
-      <c r="U34" s="2">
-        <v>6738</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21">
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -2875,14 +2747,8 @@
       <c r="S35" s="2">
         <v>500</v>
       </c>
-      <c r="T35" s="2">
-        <v>18888</v>
-      </c>
-      <c r="U35" s="2">
-        <v>19219</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21">
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
@@ -2940,14 +2806,8 @@
       <c r="S36" s="2">
         <v>500</v>
       </c>
-      <c r="T36" s="2">
-        <v>416</v>
-      </c>
-      <c r="U36" s="2">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21">
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
@@ -3005,14 +2865,8 @@
       <c r="S37" s="2">
         <v>500</v>
       </c>
-      <c r="T37" s="2">
-        <v>39958</v>
-      </c>
-      <c r="U37" s="2">
-        <v>40165</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21">
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
@@ -3070,14 +2924,8 @@
       <c r="S38" s="2">
         <v>500</v>
       </c>
-      <c r="T38" s="2">
-        <v>23639</v>
-      </c>
-      <c r="U38" s="2">
-        <v>23962</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21">
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -3135,14 +2983,8 @@
       <c r="S39" s="2">
         <v>500</v>
       </c>
-      <c r="T39" s="2">
-        <v>9501</v>
-      </c>
-      <c r="U39" s="2">
-        <v>9625</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21">
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
@@ -3200,14 +3042,8 @@
       <c r="S40" s="2">
         <v>500</v>
       </c>
-      <c r="T40" s="2">
-        <v>34014</v>
-      </c>
-      <c r="U40" s="2">
-        <v>34365</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21">
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
@@ -3265,14 +3101,8 @@
       <c r="S41" s="2">
         <v>500</v>
       </c>
-      <c r="T41" s="2">
-        <v>110171</v>
-      </c>
-      <c r="U41" s="2">
-        <v>111264</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21">
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42" s="1" t="s">
         <v>38</v>
       </c>
@@ -3330,14 +3160,8 @@
       <c r="S42" s="2">
         <v>500</v>
       </c>
-      <c r="T42" s="2">
-        <v>86716</v>
-      </c>
-      <c r="U42" s="2">
-        <v>87511</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21">
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43" s="1" t="s">
         <v>39</v>
       </c>
@@ -3395,14 +3219,8 @@
       <c r="S43" s="2">
         <v>500</v>
       </c>
-      <c r="T43" s="2">
-        <v>62842</v>
-      </c>
-      <c r="U43" s="2">
-        <v>63628</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21">
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44" s="1" t="s">
         <v>40</v>
       </c>
@@ -3460,14 +3278,8 @@
       <c r="S44" s="2">
         <v>500</v>
       </c>
-      <c r="T44" s="2">
-        <v>13832</v>
-      </c>
-      <c r="U44" s="2">
-        <v>13969</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21">
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
@@ -3525,14 +3337,8 @@
       <c r="S45" s="2">
         <v>500</v>
       </c>
-      <c r="T45" s="2">
-        <v>16938</v>
-      </c>
-      <c r="U45" s="2">
-        <v>17128</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21">
+    </row>
+    <row r="46" spans="1:19">
       <c r="A46" s="1" t="s">
         <v>42</v>
       </c>
@@ -3590,14 +3396,8 @@
       <c r="S46" s="2">
         <v>500</v>
       </c>
-      <c r="T46" s="2">
-        <v>16727</v>
-      </c>
-      <c r="U46" s="2">
-        <v>16954</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21">
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" s="1" t="s">
         <v>43</v>
       </c>
@@ -3655,14 +3455,8 @@
       <c r="S47" s="2">
         <v>500</v>
       </c>
-      <c r="T47" s="2">
-        <v>23862</v>
-      </c>
-      <c r="U47" s="2">
-        <v>24099</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21">
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" s="1" t="s">
         <v>44</v>
       </c>
@@ -3720,14 +3514,8 @@
       <c r="S48" s="2">
         <v>500</v>
       </c>
-      <c r="T48" s="2">
-        <v>31330</v>
-      </c>
-      <c r="U48" s="2">
-        <v>31722</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21">
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49" s="1" t="s">
         <v>45</v>
       </c>
@@ -3785,14 +3573,8 @@
       <c r="S49" s="2">
         <v>500</v>
       </c>
-      <c r="T49" s="2">
-        <v>72603</v>
-      </c>
-      <c r="U49" s="2">
-        <v>73158</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21">
+    </row>
+    <row r="50" spans="1:19">
       <c r="A50" s="1" t="s">
         <v>46</v>
       </c>
@@ -3850,14 +3632,8 @@
       <c r="S50" s="2">
         <v>500</v>
       </c>
-      <c r="T50" s="2">
-        <v>43240</v>
-      </c>
-      <c r="U50" s="2">
-        <v>43676</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21">
+    </row>
+    <row r="51" spans="1:19">
       <c r="A51" s="1" t="s">
         <v>47</v>
       </c>
@@ -3915,14 +3691,8 @@
       <c r="S51" s="2">
         <v>500</v>
       </c>
-      <c r="T51" s="2">
-        <v>2032</v>
-      </c>
-      <c r="U51" s="2">
-        <v>2075</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21">
+    </row>
+    <row r="52" spans="1:19">
       <c r="A52" s="1" t="s">
         <v>48</v>
       </c>
@@ -3980,14 +3750,8 @@
       <c r="S52" s="2">
         <v>500</v>
       </c>
-      <c r="T52" s="2">
-        <v>15165</v>
-      </c>
-      <c r="U52" s="2">
-        <v>15339</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21">
+    </row>
+    <row r="53" spans="1:19">
       <c r="A53" s="1" t="s">
         <v>49</v>
       </c>
@@ -4045,14 +3809,8 @@
       <c r="S53" s="2">
         <v>500</v>
       </c>
-      <c r="T53" s="2">
-        <v>153897</v>
-      </c>
-      <c r="U53" s="2">
-        <v>155916</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21">
+    </row>
+    <row r="54" spans="1:19">
       <c r="A54" s="1" t="s">
         <v>50</v>
       </c>
@@ -4110,14 +3868,8 @@
       <c r="S54" s="2">
         <v>500</v>
       </c>
-      <c r="T54" s="2">
-        <v>58135</v>
-      </c>
-      <c r="U54" s="2">
-        <v>58832</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21">
+    </row>
+    <row r="55" spans="1:19">
       <c r="A55" s="1" t="s">
         <v>51</v>
       </c>
@@ -4175,14 +3927,8 @@
       <c r="S55" s="2">
         <v>500</v>
       </c>
-      <c r="T55" s="2">
-        <v>72168</v>
-      </c>
-      <c r="U55" s="2">
-        <v>73088</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21">
+    </row>
+    <row r="56" spans="1:19">
       <c r="A56" s="1" t="s">
         <v>52</v>
       </c>
@@ -4240,14 +3986,8 @@
       <c r="S56" s="2">
         <v>500</v>
       </c>
-      <c r="T56" s="2">
-        <v>164869</v>
-      </c>
-      <c r="U56" s="2">
-        <v>166842</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21">
+    </row>
+    <row r="57" spans="1:19">
       <c r="A57" s="1" t="s">
         <v>53</v>
       </c>
@@ -4305,14 +4045,8 @@
       <c r="S57" s="2">
         <v>500</v>
       </c>
-      <c r="T57" s="2">
-        <v>136340</v>
-      </c>
-      <c r="U57" s="2">
-        <v>138166</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21">
+    </row>
+    <row r="58" spans="1:19">
       <c r="A58" s="1" t="s">
         <v>54</v>
       </c>
@@ -4370,14 +4104,8 @@
       <c r="S58" s="2">
         <v>500</v>
       </c>
-      <c r="T58" s="2">
-        <v>137231</v>
-      </c>
-      <c r="U58" s="2">
-        <v>139114</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21">
+    </row>
+    <row r="59" spans="1:19">
       <c r="A59" s="1" t="s">
         <v>55</v>
       </c>
@@ -4435,14 +4163,8 @@
       <c r="S59" s="2">
         <v>500</v>
       </c>
-      <c r="T59" s="2">
-        <v>136905</v>
-      </c>
-      <c r="U59" s="2">
-        <v>138578</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21">
+    </row>
+    <row r="60" spans="1:19">
       <c r="A60" s="1" t="s">
         <v>56</v>
       </c>
@@ -4500,14 +4222,8 @@
       <c r="S60" s="2">
         <v>500</v>
       </c>
-      <c r="T60" s="2">
-        <v>64679</v>
-      </c>
-      <c r="U60" s="2">
-        <v>65657</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21">
+    </row>
+    <row r="61" spans="1:19">
       <c r="A61" s="1" t="s">
         <v>57</v>
       </c>
@@ -4565,14 +4281,8 @@
       <c r="S61" s="2">
         <v>500</v>
       </c>
-      <c r="T61" s="2">
-        <v>5743</v>
-      </c>
-      <c r="U61" s="2">
-        <v>5845</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21">
+    </row>
+    <row r="62" spans="1:19">
       <c r="A62" s="1" t="s">
         <v>58</v>
       </c>
@@ -4629,12 +4339,6 @@
       </c>
       <c r="S62" s="2">
         <v>500</v>
-      </c>
-      <c r="T62" s="2">
-        <v>4072</v>
-      </c>
-      <c r="U62" s="2">
-        <v>4157</v>
       </c>
     </row>
   </sheetData>
@@ -4678,81 +4382,81 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="T3" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="U3" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="V3" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="W3" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="X3" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="X3" s="4" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -7421,7 +7125,7 @@
     </row>
     <row r="40" spans="1:24">
       <c r="A40" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B40" s="5">
         <v>2</v>
@@ -7495,7 +7199,7 @@
     </row>
     <row r="41" spans="1:24">
       <c r="A41" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B41" s="5">
         <v>462</v>
@@ -7643,7 +7347,7 @@
     </row>
     <row r="43" spans="1:24">
       <c r="A43" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B43" s="5">
         <v>13</v>
@@ -8009,6 +7713,2777 @@
       </c>
       <c r="X47" s="5">
         <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="8" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="8" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="8" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" style="8" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" style="8" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" style="8" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" style="8" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" style="8" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" style="8" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" style="8" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" style="8" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" style="8" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5">
+        <v>10385</v>
+      </c>
+      <c r="C4" s="7">
+        <v>100</v>
+      </c>
+      <c r="D4" s="7">
+        <v>51.5</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.17516</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.03476</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.07607</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0.21213</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.26866</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.13182</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0.04073</v>
+      </c>
+      <c r="L4" s="8">
+        <v>0.01714</v>
+      </c>
+      <c r="M4" s="8">
+        <v>0.00847</v>
+      </c>
+      <c r="N4" s="8">
+        <v>0.00664</v>
+      </c>
+      <c r="O4" s="8">
+        <v>0.0052</v>
+      </c>
+      <c r="P4" s="8">
+        <v>0.00443</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>0.00404</v>
+      </c>
+      <c r="R4" s="8">
+        <v>0.00308</v>
+      </c>
+      <c r="S4" s="8">
+        <v>0.00414</v>
+      </c>
+      <c r="T4" s="8">
+        <v>0.00212</v>
+      </c>
+      <c r="U4" s="8">
+        <v>0.00539</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5">
+        <v>21748</v>
+      </c>
+      <c r="C5" s="7">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="D5" s="7">
+        <v>26.9</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.13761</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.22804</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.21465</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.15229</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0.08895</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0.05244</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0.0343</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0.02474</v>
+      </c>
+      <c r="M5" s="8">
+        <v>0.01722</v>
+      </c>
+      <c r="N5" s="8">
+        <v>0.01048</v>
+      </c>
+      <c r="O5" s="8">
+        <v>0.009509999999999999</v>
+      </c>
+      <c r="P5" s="8">
+        <v>0.00743</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>0.00577</v>
+      </c>
+      <c r="R5" s="8">
+        <v>0.00365</v>
+      </c>
+      <c r="S5" s="8">
+        <v>0.00466</v>
+      </c>
+      <c r="T5" s="8">
+        <v>0.00328</v>
+      </c>
+      <c r="U5" s="8">
+        <v>0.00499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5">
+        <v>30528</v>
+      </c>
+      <c r="C6" s="7">
+        <v>75</v>
+      </c>
+      <c r="D6" s="7">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="E6" s="8">
+        <v>4E-05</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8">
+        <v>4E-05</v>
+      </c>
+      <c r="J6" s="8">
+        <v>4E-05</v>
+      </c>
+      <c r="K6" s="8">
+        <v>4E-05</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0</v>
+      </c>
+      <c r="M6" s="8">
+        <v>0</v>
+      </c>
+      <c r="N6" s="8">
+        <v>0</v>
+      </c>
+      <c r="O6" s="8">
+        <v>0</v>
+      </c>
+      <c r="P6" s="8">
+        <v>4E-05</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>4E-05</v>
+      </c>
+      <c r="R6" s="8">
+        <v>0.00017</v>
+      </c>
+      <c r="S6" s="8">
+        <v>0.00026</v>
+      </c>
+      <c r="T6" s="8">
+        <v>0.00048</v>
+      </c>
+      <c r="U6" s="8">
+        <v>0.99882</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
+        <v>42170</v>
+      </c>
+      <c r="C7" s="7">
+        <v>27.6</v>
+      </c>
+      <c r="D7" s="7">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.0005999999999999999</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.00138</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.00086</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.0005999999999999999</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.00034</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0.00034</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0.00026</v>
+      </c>
+      <c r="L7" s="8">
+        <v>0.00034</v>
+      </c>
+      <c r="M7" s="8">
+        <v>0.00017</v>
+      </c>
+      <c r="N7" s="8">
+        <v>0.00043</v>
+      </c>
+      <c r="O7" s="8">
+        <v>0.00017</v>
+      </c>
+      <c r="P7" s="8">
+        <v>0.00034</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>0.00069</v>
+      </c>
+      <c r="R7" s="8">
+        <v>9.000000000000001E-05</v>
+      </c>
+      <c r="S7" s="8">
+        <v>0.00043</v>
+      </c>
+      <c r="T7" s="8">
+        <v>0.00086</v>
+      </c>
+      <c r="U7" s="8">
+        <v>0.99209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5">
+        <v>218</v>
+      </c>
+      <c r="C8" s="7">
+        <v>96.3</v>
+      </c>
+      <c r="D8" s="7">
+        <v>77.59999999999999</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.07142999999999999</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.07142999999999999</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.02857</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0.02381</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.02381</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.02381</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0.02381</v>
+      </c>
+      <c r="L8" s="8">
+        <v>0.02381</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0.009520000000000001</v>
+      </c>
+      <c r="N8" s="8">
+        <v>0.00476</v>
+      </c>
+      <c r="O8" s="8">
+        <v>0.009520000000000001</v>
+      </c>
+      <c r="P8" s="8">
+        <v>0.01905</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>0.0381</v>
+      </c>
+      <c r="R8" s="8">
+        <v>0.02857</v>
+      </c>
+      <c r="S8" s="8">
+        <v>0.0619</v>
+      </c>
+      <c r="T8" s="8">
+        <v>0.06666999999999999</v>
+      </c>
+      <c r="U8" s="8">
+        <v>0.47143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5">
+        <v>11566</v>
+      </c>
+      <c r="C9" s="7">
+        <v>100</v>
+      </c>
+      <c r="D9" s="7">
+        <v>100</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0</v>
+      </c>
+      <c r="K9" s="8">
+        <v>0</v>
+      </c>
+      <c r="L9" s="8">
+        <v>0</v>
+      </c>
+      <c r="M9" s="8">
+        <v>0</v>
+      </c>
+      <c r="N9" s="8">
+        <v>9.000000000000001E-05</v>
+      </c>
+      <c r="O9" s="8">
+        <v>9.000000000000001E-05</v>
+      </c>
+      <c r="P9" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>0</v>
+      </c>
+      <c r="R9" s="8">
+        <v>9.000000000000001E-05</v>
+      </c>
+      <c r="S9" s="8">
+        <v>0.00017</v>
+      </c>
+      <c r="T9" s="8">
+        <v>0.00017</v>
+      </c>
+      <c r="U9" s="8">
+        <v>0.99939</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5">
+        <v>74742</v>
+      </c>
+      <c r="C10" s="7">
+        <v>28.5</v>
+      </c>
+      <c r="D10" s="7">
+        <v>98.90000000000001</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.00038</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.00033</v>
+      </c>
+      <c r="H10" s="8">
+        <v>0.00028</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0.00047</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0.00023</v>
+      </c>
+      <c r="K10" s="8">
+        <v>0.00033</v>
+      </c>
+      <c r="L10" s="8">
+        <v>0.00085</v>
+      </c>
+      <c r="M10" s="8">
+        <v>0.00085</v>
+      </c>
+      <c r="N10" s="8">
+        <v>0.00094</v>
+      </c>
+      <c r="O10" s="8">
+        <v>0.00117</v>
+      </c>
+      <c r="P10" s="8">
+        <v>0.00207</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>0.00333</v>
+      </c>
+      <c r="R10" s="8">
+        <v>0.00446</v>
+      </c>
+      <c r="S10" s="8">
+        <v>0.01005</v>
+      </c>
+      <c r="T10" s="8">
+        <v>0.02513</v>
+      </c>
+      <c r="U10" s="8">
+        <v>0.94913</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5">
+        <v>7760</v>
+      </c>
+      <c r="C11" s="7">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="D11" s="7">
+        <v>65.90000000000001</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.01006</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.0494</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.06023</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0.06372</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.07532999999999999</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0.08835</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0.09532</v>
+      </c>
+      <c r="L11" s="8">
+        <v>0.09532</v>
+      </c>
+      <c r="M11" s="8">
+        <v>0.09286999999999999</v>
+      </c>
+      <c r="N11" s="8">
+        <v>0.07649</v>
+      </c>
+      <c r="O11" s="8">
+        <v>0.06680999999999999</v>
+      </c>
+      <c r="P11" s="8">
+        <v>0.05843</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>0.05017</v>
+      </c>
+      <c r="R11" s="8">
+        <v>0.04411</v>
+      </c>
+      <c r="S11" s="8">
+        <v>0.03199</v>
+      </c>
+      <c r="T11" s="8">
+        <v>0.02709</v>
+      </c>
+      <c r="U11" s="8">
+        <v>0.01432</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5">
+        <v>3088</v>
+      </c>
+      <c r="C12" s="7">
+        <v>100</v>
+      </c>
+      <c r="D12" s="7">
+        <v>90.90000000000001</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.00032</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.009719999999999999</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0.009390000000000001</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0.01716</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0.02947</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0.03724</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0.05117</v>
+      </c>
+      <c r="L12" s="8">
+        <v>0.06574000000000001</v>
+      </c>
+      <c r="M12" s="8">
+        <v>0.08193</v>
+      </c>
+      <c r="N12" s="8">
+        <v>0.10654</v>
+      </c>
+      <c r="O12" s="8">
+        <v>0.10654</v>
+      </c>
+      <c r="P12" s="8">
+        <v>0.11399</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>0.1169</v>
+      </c>
+      <c r="R12" s="8">
+        <v>0.11237</v>
+      </c>
+      <c r="S12" s="8">
+        <v>0.07448</v>
+      </c>
+      <c r="T12" s="8">
+        <v>0.04858</v>
+      </c>
+      <c r="U12" s="8">
+        <v>0.01846</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5">
+        <v>11742</v>
+      </c>
+      <c r="C13" s="7">
+        <v>99.8</v>
+      </c>
+      <c r="D13" s="7">
+        <v>92.8</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.00614</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.01288</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0.009469999999999999</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0.008959999999999999</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0.01561</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0.0221</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0.02935</v>
+      </c>
+      <c r="L13" s="8">
+        <v>0.03771</v>
+      </c>
+      <c r="M13" s="8">
+        <v>0.04726</v>
+      </c>
+      <c r="N13" s="8">
+        <v>0.05656</v>
+      </c>
+      <c r="O13" s="8">
+        <v>0.06876</v>
+      </c>
+      <c r="P13" s="8">
+        <v>0.08864</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>0.11457</v>
+      </c>
+      <c r="R13" s="8">
+        <v>0.13615</v>
+      </c>
+      <c r="S13" s="8">
+        <v>0.13743</v>
+      </c>
+      <c r="T13" s="8">
+        <v>0.12523</v>
+      </c>
+      <c r="U13" s="8">
+        <v>0.08318</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5">
+        <v>9090</v>
+      </c>
+      <c r="C14" s="7">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="D14" s="7">
+        <v>77.90000000000001</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.00529</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.02544</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0.04086</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0.05132</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0.06476</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0.08623</v>
+      </c>
+      <c r="K14" s="8">
+        <v>0.10749</v>
+      </c>
+      <c r="L14" s="8">
+        <v>0.1228</v>
+      </c>
+      <c r="M14" s="8">
+        <v>0.12533</v>
+      </c>
+      <c r="N14" s="8">
+        <v>0.1065</v>
+      </c>
+      <c r="O14" s="8">
+        <v>0.08524</v>
+      </c>
+      <c r="P14" s="8">
+        <v>0.05551</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>0.04769</v>
+      </c>
+      <c r="R14" s="8">
+        <v>0.03238</v>
+      </c>
+      <c r="S14" s="8">
+        <v>0.0196</v>
+      </c>
+      <c r="T14" s="8">
+        <v>0.0141</v>
+      </c>
+      <c r="U14" s="8">
+        <v>0.009469999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="5">
+        <v>11608</v>
+      </c>
+      <c r="C15" s="7">
+        <v>100</v>
+      </c>
+      <c r="D15" s="7">
+        <v>78.3</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0.01491</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.02525</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0.03068</v>
+      </c>
+      <c r="H15" s="8">
+        <v>0.04171</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0.05523</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0.07385</v>
+      </c>
+      <c r="K15" s="8">
+        <v>0.08651</v>
+      </c>
+      <c r="L15" s="8">
+        <v>0.09668</v>
+      </c>
+      <c r="M15" s="8">
+        <v>0.09711</v>
+      </c>
+      <c r="N15" s="8">
+        <v>0.09254999999999999</v>
+      </c>
+      <c r="O15" s="8">
+        <v>0.0916</v>
+      </c>
+      <c r="P15" s="8">
+        <v>0.07376000000000001</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>0.06196</v>
+      </c>
+      <c r="R15" s="8">
+        <v>0.05437</v>
+      </c>
+      <c r="S15" s="8">
+        <v>0.04541</v>
+      </c>
+      <c r="T15" s="8">
+        <v>0.03654</v>
+      </c>
+      <c r="U15" s="8">
+        <v>0.02189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5">
+        <v>958</v>
+      </c>
+      <c r="C16" s="7">
+        <v>100</v>
+      </c>
+      <c r="D16" s="7">
+        <v>21.7</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.00209</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.1785</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0.40292</v>
+      </c>
+      <c r="H16" s="8">
+        <v>0.17328</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0.05428</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0.02505</v>
+      </c>
+      <c r="K16" s="8">
+        <v>0.01461</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0.01357</v>
+      </c>
+      <c r="M16" s="8">
+        <v>0.01253</v>
+      </c>
+      <c r="N16" s="8">
+        <v>0.00835</v>
+      </c>
+      <c r="O16" s="8">
+        <v>0.00626</v>
+      </c>
+      <c r="P16" s="8">
+        <v>0.00522</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>0.01044</v>
+      </c>
+      <c r="R16" s="8">
+        <v>0.00835</v>
+      </c>
+      <c r="S16" s="8">
+        <v>0.00313</v>
+      </c>
+      <c r="T16" s="8">
+        <v>0.009390000000000001</v>
+      </c>
+      <c r="U16" s="8">
+        <v>0.07203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="5">
+        <v>25416</v>
+      </c>
+      <c r="C17" s="7">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="D17" s="7">
+        <v>99.7</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.00016</v>
+      </c>
+      <c r="G17" s="8">
+        <v>8.000000000000001E-05</v>
+      </c>
+      <c r="H17" s="8">
+        <v>4E-05</v>
+      </c>
+      <c r="I17" s="8">
+        <v>8.000000000000001E-05</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0.00016</v>
+      </c>
+      <c r="K17" s="8">
+        <v>4E-05</v>
+      </c>
+      <c r="L17" s="8">
+        <v>0.00016</v>
+      </c>
+      <c r="M17" s="8">
+        <v>8.000000000000001E-05</v>
+      </c>
+      <c r="N17" s="8">
+        <v>0.00016</v>
+      </c>
+      <c r="O17" s="8">
+        <v>0.00024</v>
+      </c>
+      <c r="P17" s="8">
+        <v>0.00035</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>0.00043</v>
+      </c>
+      <c r="R17" s="8">
+        <v>0.00055</v>
+      </c>
+      <c r="S17" s="8">
+        <v>0.00126</v>
+      </c>
+      <c r="T17" s="8">
+        <v>0.00433</v>
+      </c>
+      <c r="U17" s="8">
+        <v>0.99189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="5">
+        <v>4964</v>
+      </c>
+      <c r="C18" s="7">
+        <v>99.8</v>
+      </c>
+      <c r="D18" s="7">
+        <v>31.5</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0.18006</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0.35567</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0.11788</v>
+      </c>
+      <c r="H18" s="8">
+        <v>0.05773</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0.02786</v>
+      </c>
+      <c r="J18" s="8">
+        <v>0.01776</v>
+      </c>
+      <c r="K18" s="8">
+        <v>0.01151</v>
+      </c>
+      <c r="L18" s="8">
+        <v>0.00929</v>
+      </c>
+      <c r="M18" s="8">
+        <v>0.00706</v>
+      </c>
+      <c r="N18" s="8">
+        <v>0.00747</v>
+      </c>
+      <c r="O18" s="8">
+        <v>0.00929</v>
+      </c>
+      <c r="P18" s="8">
+        <v>0.00666</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>0.008070000000000001</v>
+      </c>
+      <c r="R18" s="8">
+        <v>0.01151</v>
+      </c>
+      <c r="S18" s="8">
+        <v>0.0113</v>
+      </c>
+      <c r="T18" s="8">
+        <v>0.01453</v>
+      </c>
+      <c r="U18" s="8">
+        <v>0.14635</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="5">
+        <v>91830</v>
+      </c>
+      <c r="C19" s="7">
+        <v>10.2</v>
+      </c>
+      <c r="D19" s="7">
+        <v>96.90000000000001</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0.00021</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0.00224</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.00106</v>
+      </c>
+      <c r="H19" s="8">
+        <v>0.00277</v>
+      </c>
+      <c r="I19" s="8">
+        <v>0.00256</v>
+      </c>
+      <c r="J19" s="8">
+        <v>0.0017</v>
+      </c>
+      <c r="K19" s="8">
+        <v>0.00319</v>
+      </c>
+      <c r="L19" s="8">
+        <v>0.00479</v>
+      </c>
+      <c r="M19" s="8">
+        <v>0.00735</v>
+      </c>
+      <c r="N19" s="8">
+        <v>0.009480000000000001</v>
+      </c>
+      <c r="O19" s="8">
+        <v>0.01171</v>
+      </c>
+      <c r="P19" s="8">
+        <v>0.01725</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>0.02268</v>
+      </c>
+      <c r="R19" s="8">
+        <v>0.03706</v>
+      </c>
+      <c r="S19" s="8">
+        <v>0.04771</v>
+      </c>
+      <c r="T19" s="8">
+        <v>0.09701</v>
+      </c>
+      <c r="U19" s="8">
+        <v>0.73123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="5">
+        <v>13910</v>
+      </c>
+      <c r="C20" s="7">
+        <v>100</v>
+      </c>
+      <c r="D20" s="7">
+        <v>84.2</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0.00374</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0.009350000000000001</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.01453</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0.01316</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0.01524</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0.01381</v>
+      </c>
+      <c r="K20" s="8">
+        <v>0.01481</v>
+      </c>
+      <c r="L20" s="8">
+        <v>0.02006</v>
+      </c>
+      <c r="M20" s="8">
+        <v>0.02337</v>
+      </c>
+      <c r="N20" s="8">
+        <v>0.02826</v>
+      </c>
+      <c r="O20" s="8">
+        <v>0.03912</v>
+      </c>
+      <c r="P20" s="8">
+        <v>0.05213</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>0.07529</v>
+      </c>
+      <c r="R20" s="8">
+        <v>0.11361</v>
+      </c>
+      <c r="S20" s="8">
+        <v>0.1372</v>
+      </c>
+      <c r="T20" s="8">
+        <v>0.17603</v>
+      </c>
+      <c r="U20" s="8">
+        <v>0.25031</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="5">
+        <v>3276</v>
+      </c>
+      <c r="C21" s="7">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="D21" s="7">
+        <v>98</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0.00458</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0.00305</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0.00122</v>
+      </c>
+      <c r="H21" s="8">
+        <v>0.00061</v>
+      </c>
+      <c r="I21" s="8">
+        <v>0.00275</v>
+      </c>
+      <c r="J21" s="8">
+        <v>0.00214</v>
+      </c>
+      <c r="K21" s="8">
+        <v>0.00305</v>
+      </c>
+      <c r="L21" s="8">
+        <v>0.00336</v>
+      </c>
+      <c r="M21" s="8">
+        <v>0.00703</v>
+      </c>
+      <c r="N21" s="8">
+        <v>0.01222</v>
+      </c>
+      <c r="O21" s="8">
+        <v>0.01802</v>
+      </c>
+      <c r="P21" s="8">
+        <v>0.01772</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>0.02841</v>
+      </c>
+      <c r="R21" s="8">
+        <v>0.04307</v>
+      </c>
+      <c r="S21" s="8">
+        <v>0.0675</v>
+      </c>
+      <c r="T21" s="8">
+        <v>0.16952</v>
+      </c>
+      <c r="U21" s="8">
+        <v>0.61576</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="5">
+        <v>17171</v>
+      </c>
+      <c r="C22" s="7">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="D22" s="7">
+        <v>73.09999999999999</v>
+      </c>
+      <c r="E22" s="8">
+        <v>0.009560000000000001</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0.04761</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.05314</v>
+      </c>
+      <c r="H22" s="8">
+        <v>0.06509</v>
+      </c>
+      <c r="I22" s="8">
+        <v>0.07249</v>
+      </c>
+      <c r="J22" s="8">
+        <v>0.08903</v>
+      </c>
+      <c r="K22" s="8">
+        <v>0.09614</v>
+      </c>
+      <c r="L22" s="8">
+        <v>0.10465</v>
+      </c>
+      <c r="M22" s="8">
+        <v>0.10547</v>
+      </c>
+      <c r="N22" s="8">
+        <v>0.09224</v>
+      </c>
+      <c r="O22" s="8">
+        <v>0.07633</v>
+      </c>
+      <c r="P22" s="8">
+        <v>0.05734</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>0.04265</v>
+      </c>
+      <c r="R22" s="8">
+        <v>0.03123</v>
+      </c>
+      <c r="S22" s="8">
+        <v>0.02307</v>
+      </c>
+      <c r="T22" s="8">
+        <v>0.02051</v>
+      </c>
+      <c r="U22" s="8">
+        <v>0.01346</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="A23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="5">
+        <v>7854</v>
+      </c>
+      <c r="C23" s="7">
+        <v>100</v>
+      </c>
+      <c r="D23" s="7">
+        <v>93.90000000000001</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0.00484</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0.01452</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0.01032</v>
+      </c>
+      <c r="H23" s="8">
+        <v>0.008920000000000001</v>
+      </c>
+      <c r="I23" s="8">
+        <v>0.0107</v>
+      </c>
+      <c r="J23" s="8">
+        <v>0.01452</v>
+      </c>
+      <c r="K23" s="8">
+        <v>0.02254</v>
+      </c>
+      <c r="L23" s="8">
+        <v>0.03133</v>
+      </c>
+      <c r="M23" s="8">
+        <v>0.05095</v>
+      </c>
+      <c r="N23" s="8">
+        <v>0.06063</v>
+      </c>
+      <c r="O23" s="8">
+        <v>0.07974000000000001</v>
+      </c>
+      <c r="P23" s="8">
+        <v>0.10699</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>0.15578</v>
+      </c>
+      <c r="R23" s="8">
+        <v>0.20431</v>
+      </c>
+      <c r="S23" s="8">
+        <v>0.14495</v>
+      </c>
+      <c r="T23" s="8">
+        <v>0.05439</v>
+      </c>
+      <c r="U23" s="8">
+        <v>0.02458</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="A24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="5">
+        <v>7194</v>
+      </c>
+      <c r="C24" s="7">
+        <v>100</v>
+      </c>
+      <c r="D24" s="7">
+        <v>82.90000000000001</v>
+      </c>
+      <c r="E24" s="8">
+        <v>0.009039999999999999</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.03725</v>
+      </c>
+      <c r="G24" s="8">
+        <v>0.02349</v>
+      </c>
+      <c r="H24" s="8">
+        <v>0.02613</v>
+      </c>
+      <c r="I24" s="8">
+        <v>0.0367</v>
+      </c>
+      <c r="J24" s="8">
+        <v>0.04518</v>
+      </c>
+      <c r="K24" s="8">
+        <v>0.05616</v>
+      </c>
+      <c r="L24" s="8">
+        <v>0.07131</v>
+      </c>
+      <c r="M24" s="8">
+        <v>0.08742999999999999</v>
+      </c>
+      <c r="N24" s="8">
+        <v>0.08604000000000001</v>
+      </c>
+      <c r="O24" s="8">
+        <v>0.09425</v>
+      </c>
+      <c r="P24" s="8">
+        <v>0.08869</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>0.07464999999999999</v>
+      </c>
+      <c r="R24" s="8">
+        <v>0.0752</v>
+      </c>
+      <c r="S24" s="8">
+        <v>0.06950000000000001</v>
+      </c>
+      <c r="T24" s="8">
+        <v>0.07145</v>
+      </c>
+      <c r="U24" s="8">
+        <v>0.04754</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="A25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="5">
+        <v>11757</v>
+      </c>
+      <c r="C25" s="7">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="D25" s="7">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="E25" s="8">
+        <v>9.000000000000001E-05</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.00026</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0.00017</v>
+      </c>
+      <c r="H25" s="8">
+        <v>0.00017</v>
+      </c>
+      <c r="I25" s="8">
+        <v>0.00034</v>
+      </c>
+      <c r="J25" s="8">
+        <v>0.00017</v>
+      </c>
+      <c r="K25" s="8">
+        <v>0.00077</v>
+      </c>
+      <c r="L25" s="8">
+        <v>0.00068</v>
+      </c>
+      <c r="M25" s="8">
+        <v>0.00136</v>
+      </c>
+      <c r="N25" s="8">
+        <v>0.00136</v>
+      </c>
+      <c r="O25" s="8">
+        <v>0.00213</v>
+      </c>
+      <c r="P25" s="8">
+        <v>0.004</v>
+      </c>
+      <c r="Q25" s="8">
+        <v>0.00477</v>
+      </c>
+      <c r="R25" s="8">
+        <v>0.00817</v>
+      </c>
+      <c r="S25" s="8">
+        <v>0.01455</v>
+      </c>
+      <c r="T25" s="8">
+        <v>0.04281</v>
+      </c>
+      <c r="U25" s="8">
+        <v>0.91821</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="5">
+        <v>719</v>
+      </c>
+      <c r="C26" s="7">
+        <v>96</v>
+      </c>
+      <c r="D26" s="7">
+        <v>58.7</v>
+      </c>
+      <c r="E26" s="8">
+        <v>0.28261</v>
+      </c>
+      <c r="F26" s="8">
+        <v>0.05507</v>
+      </c>
+      <c r="G26" s="8">
+        <v>0.03913</v>
+      </c>
+      <c r="H26" s="8">
+        <v>0.01739</v>
+      </c>
+      <c r="I26" s="8">
+        <v>0.03188</v>
+      </c>
+      <c r="J26" s="8">
+        <v>0.03188</v>
+      </c>
+      <c r="K26" s="8">
+        <v>0.02029</v>
+      </c>
+      <c r="L26" s="8">
+        <v>0.02319</v>
+      </c>
+      <c r="M26" s="8">
+        <v>0.01739</v>
+      </c>
+      <c r="N26" s="8">
+        <v>0.02319</v>
+      </c>
+      <c r="O26" s="8">
+        <v>0.02029</v>
+      </c>
+      <c r="P26" s="8">
+        <v>0.01304</v>
+      </c>
+      <c r="Q26" s="8">
+        <v>0.01739</v>
+      </c>
+      <c r="R26" s="8">
+        <v>0.01594</v>
+      </c>
+      <c r="S26" s="8">
+        <v>0.01449</v>
+      </c>
+      <c r="T26" s="8">
+        <v>0.02029</v>
+      </c>
+      <c r="U26" s="8">
+        <v>0.35652</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="5">
+        <v>34736</v>
+      </c>
+      <c r="C27" s="7">
+        <v>63.7</v>
+      </c>
+      <c r="D27" s="7">
+        <v>99.7</v>
+      </c>
+      <c r="E27" s="8">
+        <v>0</v>
+      </c>
+      <c r="F27" s="8">
+        <v>5E-05</v>
+      </c>
+      <c r="G27" s="8">
+        <v>9.000000000000001E-05</v>
+      </c>
+      <c r="H27" s="8">
+        <v>0</v>
+      </c>
+      <c r="I27" s="8">
+        <v>5E-05</v>
+      </c>
+      <c r="J27" s="8">
+        <v>0.00018</v>
+      </c>
+      <c r="K27" s="8">
+        <v>0.00023</v>
+      </c>
+      <c r="L27" s="8">
+        <v>0.00027</v>
+      </c>
+      <c r="M27" s="8">
+        <v>0.00032</v>
+      </c>
+      <c r="N27" s="8">
+        <v>0.00063</v>
+      </c>
+      <c r="O27" s="8">
+        <v>0.00113</v>
+      </c>
+      <c r="P27" s="8">
+        <v>0.00235</v>
+      </c>
+      <c r="Q27" s="8">
+        <v>0.00289</v>
+      </c>
+      <c r="R27" s="8">
+        <v>0.00682</v>
+      </c>
+      <c r="S27" s="8">
+        <v>0.01631</v>
+      </c>
+      <c r="T27" s="8">
+        <v>0.05728</v>
+      </c>
+      <c r="U27" s="8">
+        <v>0.91142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="5">
+        <v>16963</v>
+      </c>
+      <c r="C28" s="7">
+        <v>100</v>
+      </c>
+      <c r="D28" s="7">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="E28" s="8">
+        <v>0.00012</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.00065</v>
+      </c>
+      <c r="G28" s="8">
+        <v>0.00035</v>
+      </c>
+      <c r="H28" s="8">
+        <v>0.00035</v>
+      </c>
+      <c r="I28" s="8">
+        <v>0.00024</v>
+      </c>
+      <c r="J28" s="8">
+        <v>0.00035</v>
+      </c>
+      <c r="K28" s="8">
+        <v>0.00088</v>
+      </c>
+      <c r="L28" s="8">
+        <v>0.00124</v>
+      </c>
+      <c r="M28" s="8">
+        <v>0.00112</v>
+      </c>
+      <c r="N28" s="8">
+        <v>0.00124</v>
+      </c>
+      <c r="O28" s="8">
+        <v>0.00177</v>
+      </c>
+      <c r="P28" s="8">
+        <v>0.00236</v>
+      </c>
+      <c r="Q28" s="8">
+        <v>0.0043</v>
+      </c>
+      <c r="R28" s="8">
+        <v>0.00843</v>
+      </c>
+      <c r="S28" s="8">
+        <v>0.01604</v>
+      </c>
+      <c r="T28" s="8">
+        <v>0.04788</v>
+      </c>
+      <c r="U28" s="8">
+        <v>0.91267</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="5">
+        <v>6451</v>
+      </c>
+      <c r="C29" s="7">
+        <v>99.8</v>
+      </c>
+      <c r="D29" s="7">
+        <v>99.5</v>
+      </c>
+      <c r="E29" s="8">
+        <v>0.00233</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0.00047</v>
+      </c>
+      <c r="G29" s="8">
+        <v>0.00047</v>
+      </c>
+      <c r="H29" s="8">
+        <v>0.00047</v>
+      </c>
+      <c r="I29" s="8">
+        <v>0.00016</v>
+      </c>
+      <c r="J29" s="8">
+        <v>0.00016</v>
+      </c>
+      <c r="K29" s="8">
+        <v>0.0009300000000000001</v>
+      </c>
+      <c r="L29" s="8">
+        <v>0.00233</v>
+      </c>
+      <c r="M29" s="8">
+        <v>0.00466</v>
+      </c>
+      <c r="N29" s="8">
+        <v>0.00559</v>
+      </c>
+      <c r="O29" s="8">
+        <v>0.008229999999999999</v>
+      </c>
+      <c r="P29" s="8">
+        <v>0.01739</v>
+      </c>
+      <c r="Q29" s="8">
+        <v>0.02888</v>
+      </c>
+      <c r="R29" s="8">
+        <v>0.05061</v>
+      </c>
+      <c r="S29" s="8">
+        <v>0.08819</v>
+      </c>
+      <c r="T29" s="8">
+        <v>0.16457</v>
+      </c>
+      <c r="U29" s="8">
+        <v>0.62459</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="5">
+        <v>25878</v>
+      </c>
+      <c r="C30" s="7">
+        <v>89.90000000000001</v>
+      </c>
+      <c r="D30" s="7">
+        <v>98.90000000000001</v>
+      </c>
+      <c r="E30" s="8">
+        <v>0.00013</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0.00039</v>
+      </c>
+      <c r="G30" s="8">
+        <v>0.00086</v>
+      </c>
+      <c r="H30" s="8">
+        <v>0.0005999999999999999</v>
+      </c>
+      <c r="I30" s="8">
+        <v>0.0009</v>
+      </c>
+      <c r="J30" s="8">
+        <v>0.00107</v>
+      </c>
+      <c r="K30" s="8">
+        <v>0.00116</v>
+      </c>
+      <c r="L30" s="8">
+        <v>0.00193</v>
+      </c>
+      <c r="M30" s="8">
+        <v>0.00297</v>
+      </c>
+      <c r="N30" s="8">
+        <v>0.00284</v>
+      </c>
+      <c r="O30" s="8">
+        <v>0.00524</v>
+      </c>
+      <c r="P30" s="8">
+        <v>0.00726</v>
+      </c>
+      <c r="Q30" s="8">
+        <v>0.01212</v>
+      </c>
+      <c r="R30" s="8">
+        <v>0.01878</v>
+      </c>
+      <c r="S30" s="8">
+        <v>0.03426</v>
+      </c>
+      <c r="T30" s="8">
+        <v>0.09087000000000001</v>
+      </c>
+      <c r="U30" s="8">
+        <v>0.8186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="5">
+        <v>64304</v>
+      </c>
+      <c r="C31" s="7">
+        <v>23.4</v>
+      </c>
+      <c r="D31" s="7">
+        <v>95.3</v>
+      </c>
+      <c r="E31" s="8">
+        <v>0.00033</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0.00193</v>
+      </c>
+      <c r="G31" s="8">
+        <v>0.00326</v>
+      </c>
+      <c r="H31" s="8">
+        <v>0.00366</v>
+      </c>
+      <c r="I31" s="8">
+        <v>0.00579</v>
+      </c>
+      <c r="J31" s="8">
+        <v>0.00712</v>
+      </c>
+      <c r="K31" s="8">
+        <v>0.00851</v>
+      </c>
+      <c r="L31" s="8">
+        <v>0.01124</v>
+      </c>
+      <c r="M31" s="8">
+        <v>0.01789</v>
+      </c>
+      <c r="N31" s="8">
+        <v>0.02234</v>
+      </c>
+      <c r="O31" s="8">
+        <v>0.03019</v>
+      </c>
+      <c r="P31" s="8">
+        <v>0.04163</v>
+      </c>
+      <c r="Q31" s="8">
+        <v>0.05427</v>
+      </c>
+      <c r="R31" s="8">
+        <v>0.08167000000000001</v>
+      </c>
+      <c r="S31" s="8">
+        <v>0.11305</v>
+      </c>
+      <c r="T31" s="8">
+        <v>0.19705</v>
+      </c>
+      <c r="U31" s="8">
+        <v>0.40008</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="5">
+        <v>59739</v>
+      </c>
+      <c r="C32" s="7">
+        <v>64.90000000000001</v>
+      </c>
+      <c r="D32" s="7">
+        <v>88.3</v>
+      </c>
+      <c r="E32" s="8">
+        <v>0.01291</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0.01838</v>
+      </c>
+      <c r="G32" s="8">
+        <v>0.02423</v>
+      </c>
+      <c r="H32" s="8">
+        <v>0.01892</v>
+      </c>
+      <c r="I32" s="8">
+        <v>0.009900000000000001</v>
+      </c>
+      <c r="J32" s="8">
+        <v>0.00644</v>
+      </c>
+      <c r="K32" s="8">
+        <v>0.0042</v>
+      </c>
+      <c r="L32" s="8">
+        <v>0.00356</v>
+      </c>
+      <c r="M32" s="8">
+        <v>0.00307</v>
+      </c>
+      <c r="N32" s="8">
+        <v>0.00322</v>
+      </c>
+      <c r="O32" s="8">
+        <v>0.0032</v>
+      </c>
+      <c r="P32" s="8">
+        <v>0.00348</v>
+      </c>
+      <c r="Q32" s="8">
+        <v>0.00356</v>
+      </c>
+      <c r="R32" s="8">
+        <v>0.00467</v>
+      </c>
+      <c r="S32" s="8">
+        <v>0.008580000000000001</v>
+      </c>
+      <c r="T32" s="8">
+        <v>0.01982</v>
+      </c>
+      <c r="U32" s="8">
+        <v>0.85187</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
+      <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="5">
+        <v>39012</v>
+      </c>
+      <c r="C33" s="7">
+        <v>37.3</v>
+      </c>
+      <c r="D33" s="7">
+        <v>94.8</v>
+      </c>
+      <c r="E33" s="8">
+        <v>0.00076</v>
+      </c>
+      <c r="F33" s="8">
+        <v>0.00186</v>
+      </c>
+      <c r="G33" s="8">
+        <v>0.00241</v>
+      </c>
+      <c r="H33" s="8">
+        <v>0.00261</v>
+      </c>
+      <c r="I33" s="8">
+        <v>0.0042</v>
+      </c>
+      <c r="J33" s="8">
+        <v>0.00592</v>
+      </c>
+      <c r="K33" s="8">
+        <v>0.00592</v>
+      </c>
+      <c r="L33" s="8">
+        <v>0.00709</v>
+      </c>
+      <c r="M33" s="8">
+        <v>0.01039</v>
+      </c>
+      <c r="N33" s="8">
+        <v>0.01321</v>
+      </c>
+      <c r="O33" s="8">
+        <v>0.0152</v>
+      </c>
+      <c r="P33" s="8">
+        <v>0.01878</v>
+      </c>
+      <c r="Q33" s="8">
+        <v>0.02924</v>
+      </c>
+      <c r="R33" s="8">
+        <v>0.04265</v>
+      </c>
+      <c r="S33" s="8">
+        <v>0.06741999999999999</v>
+      </c>
+      <c r="T33" s="8">
+        <v>0.14364</v>
+      </c>
+      <c r="U33" s="8">
+        <v>0.62871</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="A34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="5">
+        <v>13818</v>
+      </c>
+      <c r="C34" s="7">
+        <v>99.40000000000001</v>
+      </c>
+      <c r="D34" s="7">
+        <v>52.8</v>
+      </c>
+      <c r="E34" s="8">
+        <v>0.11811</v>
+      </c>
+      <c r="F34" s="8">
+        <v>0.19299</v>
+      </c>
+      <c r="G34" s="8">
+        <v>0.11323</v>
+      </c>
+      <c r="H34" s="8">
+        <v>0.08318</v>
+      </c>
+      <c r="I34" s="8">
+        <v>0.06637</v>
+      </c>
+      <c r="J34" s="8">
+        <v>0.05181</v>
+      </c>
+      <c r="K34" s="8">
+        <v>0.03537</v>
+      </c>
+      <c r="L34" s="8">
+        <v>0.03093</v>
+      </c>
+      <c r="M34" s="8">
+        <v>0.02241</v>
+      </c>
+      <c r="N34" s="8">
+        <v>0.01645</v>
+      </c>
+      <c r="O34" s="8">
+        <v>0.01659</v>
+      </c>
+      <c r="P34" s="8">
+        <v>0.01368</v>
+      </c>
+      <c r="Q34" s="8">
+        <v>0.02023</v>
+      </c>
+      <c r="R34" s="8">
+        <v>0.02838</v>
+      </c>
+      <c r="S34" s="8">
+        <v>0.0465</v>
+      </c>
+      <c r="T34" s="8">
+        <v>0.07634000000000001</v>
+      </c>
+      <c r="U34" s="8">
+        <v>0.06746000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
+      <c r="A35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="5">
+        <v>14946</v>
+      </c>
+      <c r="C35" s="7">
+        <v>100</v>
+      </c>
+      <c r="D35" s="7">
+        <v>99.09999999999999</v>
+      </c>
+      <c r="E35" s="8">
+        <v>6.999999999999999E-05</v>
+      </c>
+      <c r="F35" s="8">
+        <v>0.0008</v>
+      </c>
+      <c r="G35" s="8">
+        <v>0.00107</v>
+      </c>
+      <c r="H35" s="8">
+        <v>0.0012</v>
+      </c>
+      <c r="I35" s="8">
+        <v>0.00234</v>
+      </c>
+      <c r="J35" s="8">
+        <v>0.00288</v>
+      </c>
+      <c r="K35" s="8">
+        <v>0.00442</v>
+      </c>
+      <c r="L35" s="8">
+        <v>0.00729</v>
+      </c>
+      <c r="M35" s="8">
+        <v>0.01225</v>
+      </c>
+      <c r="N35" s="8">
+        <v>0.01546</v>
+      </c>
+      <c r="O35" s="8">
+        <v>0.02443</v>
+      </c>
+      <c r="P35" s="8">
+        <v>0.03848</v>
+      </c>
+      <c r="Q35" s="8">
+        <v>0.06257</v>
+      </c>
+      <c r="R35" s="8">
+        <v>0.10333</v>
+      </c>
+      <c r="S35" s="8">
+        <v>0.17319</v>
+      </c>
+      <c r="T35" s="8">
+        <v>0.30268</v>
+      </c>
+      <c r="U35" s="8">
+        <v>0.24754</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
+      <c r="A36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="5">
+        <v>13991</v>
+      </c>
+      <c r="C36" s="7">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="D36" s="7">
+        <v>93.8</v>
+      </c>
+      <c r="E36" s="8">
+        <v>0.00143</v>
+      </c>
+      <c r="F36" s="8">
+        <v>0.00608</v>
+      </c>
+      <c r="G36" s="8">
+        <v>0.008160000000000001</v>
+      </c>
+      <c r="H36" s="8">
+        <v>0.00737</v>
+      </c>
+      <c r="I36" s="8">
+        <v>0.01345</v>
+      </c>
+      <c r="J36" s="8">
+        <v>0.01645</v>
+      </c>
+      <c r="K36" s="8">
+        <v>0.02082</v>
+      </c>
+      <c r="L36" s="8">
+        <v>0.02361</v>
+      </c>
+      <c r="M36" s="8">
+        <v>0.02983</v>
+      </c>
+      <c r="N36" s="8">
+        <v>0.0309</v>
+      </c>
+      <c r="O36" s="8">
+        <v>0.0362</v>
+      </c>
+      <c r="P36" s="8">
+        <v>0.04335</v>
+      </c>
+      <c r="Q36" s="8">
+        <v>0.06166</v>
+      </c>
+      <c r="R36" s="8">
+        <v>0.10072</v>
+      </c>
+      <c r="S36" s="8">
+        <v>0.142</v>
+      </c>
+      <c r="T36" s="8">
+        <v>0.21518</v>
+      </c>
+      <c r="U36" s="8">
+        <v>0.24279</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
+      <c r="A37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="5">
+        <v>23670</v>
+      </c>
+      <c r="C37" s="7">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="D37" s="7">
+        <v>95.3</v>
+      </c>
+      <c r="E37" s="8">
+        <v>0.00135</v>
+      </c>
+      <c r="F37" s="8">
+        <v>0.00397</v>
+      </c>
+      <c r="G37" s="8">
+        <v>0.00588</v>
+      </c>
+      <c r="H37" s="8">
+        <v>0.009339999999999999</v>
+      </c>
+      <c r="I37" s="8">
+        <v>0.01234</v>
+      </c>
+      <c r="J37" s="8">
+        <v>0.01945</v>
+      </c>
+      <c r="K37" s="8">
+        <v>0.02435</v>
+      </c>
+      <c r="L37" s="8">
+        <v>0.03323</v>
+      </c>
+      <c r="M37" s="8">
+        <v>0.04747</v>
+      </c>
+      <c r="N37" s="8">
+        <v>0.05276</v>
+      </c>
+      <c r="O37" s="8">
+        <v>0.07267</v>
+      </c>
+      <c r="P37" s="8">
+        <v>0.07981000000000001</v>
+      </c>
+      <c r="Q37" s="8">
+        <v>0.10086</v>
+      </c>
+      <c r="R37" s="8">
+        <v>0.11655</v>
+      </c>
+      <c r="S37" s="8">
+        <v>0.13823</v>
+      </c>
+      <c r="T37" s="8">
+        <v>0.17273</v>
+      </c>
+      <c r="U37" s="8">
+        <v>0.10902</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
+      <c r="A38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="5">
+        <v>21483</v>
+      </c>
+      <c r="C38" s="7">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="D38" s="7">
+        <v>92.8</v>
+      </c>
+      <c r="E38" s="8">
+        <v>0.00135</v>
+      </c>
+      <c r="F38" s="8">
+        <v>0.0089</v>
+      </c>
+      <c r="G38" s="8">
+        <v>0.0136</v>
+      </c>
+      <c r="H38" s="8">
+        <v>0.01979</v>
+      </c>
+      <c r="I38" s="8">
+        <v>0.02729</v>
+      </c>
+      <c r="J38" s="8">
+        <v>0.03288</v>
+      </c>
+      <c r="K38" s="8">
+        <v>0.0374</v>
+      </c>
+      <c r="L38" s="8">
+        <v>0.04499</v>
+      </c>
+      <c r="M38" s="8">
+        <v>0.05263</v>
+      </c>
+      <c r="N38" s="8">
+        <v>0.05803</v>
+      </c>
+      <c r="O38" s="8">
+        <v>0.06827</v>
+      </c>
+      <c r="P38" s="8">
+        <v>0.07661</v>
+      </c>
+      <c r="Q38" s="8">
+        <v>0.09072</v>
+      </c>
+      <c r="R38" s="8">
+        <v>0.10628</v>
+      </c>
+      <c r="S38" s="8">
+        <v>0.12719</v>
+      </c>
+      <c r="T38" s="8">
+        <v>0.14382</v>
+      </c>
+      <c r="U38" s="8">
+        <v>0.09026000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="A39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="5">
+        <v>52483</v>
+      </c>
+      <c r="C39" s="7">
+        <v>82.8</v>
+      </c>
+      <c r="D39" s="7">
+        <v>98.5</v>
+      </c>
+      <c r="E39" s="8">
+        <v>0.00044</v>
+      </c>
+      <c r="F39" s="8">
+        <v>0.0009</v>
+      </c>
+      <c r="G39" s="8">
+        <v>0.00081</v>
+      </c>
+      <c r="H39" s="8">
+        <v>0.00092</v>
+      </c>
+      <c r="I39" s="8">
+        <v>0.00138</v>
+      </c>
+      <c r="J39" s="8">
+        <v>0.00136</v>
+      </c>
+      <c r="K39" s="8">
+        <v>0.00221</v>
+      </c>
+      <c r="L39" s="8">
+        <v>0.00309</v>
+      </c>
+      <c r="M39" s="8">
+        <v>0.0041</v>
+      </c>
+      <c r="N39" s="8">
+        <v>0.00465</v>
+      </c>
+      <c r="O39" s="8">
+        <v>0.00675</v>
+      </c>
+      <c r="P39" s="8">
+        <v>0.00903</v>
+      </c>
+      <c r="Q39" s="8">
+        <v>0.01372</v>
+      </c>
+      <c r="R39" s="8">
+        <v>0.02084</v>
+      </c>
+      <c r="S39" s="8">
+        <v>0.03939</v>
+      </c>
+      <c r="T39" s="8">
+        <v>0.09564</v>
+      </c>
+      <c r="U39" s="8">
+        <v>0.79479</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
+      <c r="A40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="5">
+        <v>30261</v>
+      </c>
+      <c r="C40" s="7">
+        <v>65.7</v>
+      </c>
+      <c r="D40" s="7">
+        <v>99.7</v>
+      </c>
+      <c r="E40" s="8">
+        <v>5E-05</v>
+      </c>
+      <c r="F40" s="8">
+        <v>5E-05</v>
+      </c>
+      <c r="G40" s="8">
+        <v>0</v>
+      </c>
+      <c r="H40" s="8">
+        <v>5E-05</v>
+      </c>
+      <c r="I40" s="8">
+        <v>0.0002</v>
+      </c>
+      <c r="J40" s="8">
+        <v>5E-05</v>
+      </c>
+      <c r="K40" s="8">
+        <v>5E-05</v>
+      </c>
+      <c r="L40" s="8">
+        <v>0.0001</v>
+      </c>
+      <c r="M40" s="8">
+        <v>0.0002</v>
+      </c>
+      <c r="N40" s="8">
+        <v>0</v>
+      </c>
+      <c r="O40" s="8">
+        <v>0.0004</v>
+      </c>
+      <c r="P40" s="8">
+        <v>0.00055</v>
+      </c>
+      <c r="Q40" s="8">
+        <v>0.0005999999999999999</v>
+      </c>
+      <c r="R40" s="8">
+        <v>0.00111</v>
+      </c>
+      <c r="S40" s="8">
+        <v>0.00251</v>
+      </c>
+      <c r="T40" s="8">
+        <v>0.00699</v>
+      </c>
+      <c r="U40" s="8">
+        <v>0.98708</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
+      <c r="A41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="5">
+        <v>858</v>
+      </c>
+      <c r="C41" s="7">
+        <v>100</v>
+      </c>
+      <c r="D41" s="7">
+        <v>95</v>
+      </c>
+      <c r="E41" s="8">
+        <v>0.0035</v>
+      </c>
+      <c r="F41" s="8">
+        <v>0.01049</v>
+      </c>
+      <c r="G41" s="8">
+        <v>0.01632</v>
+      </c>
+      <c r="H41" s="8">
+        <v>0.01748</v>
+      </c>
+      <c r="I41" s="8">
+        <v>0.00233</v>
+      </c>
+      <c r="J41" s="8">
+        <v>0.00466</v>
+      </c>
+      <c r="K41" s="8">
+        <v>0.00117</v>
+      </c>
+      <c r="L41" s="8">
+        <v>0.00117</v>
+      </c>
+      <c r="M41" s="8">
+        <v>0.00117</v>
+      </c>
+      <c r="N41" s="8">
+        <v>0</v>
+      </c>
+      <c r="O41" s="8">
+        <v>0.00117</v>
+      </c>
+      <c r="P41" s="8">
+        <v>0.00233</v>
+      </c>
+      <c r="Q41" s="8">
+        <v>0.00117</v>
+      </c>
+      <c r="R41" s="8">
+        <v>0.00233</v>
+      </c>
+      <c r="S41" s="8">
+        <v>0.00117</v>
+      </c>
+      <c r="T41" s="8">
+        <v>0.0035</v>
+      </c>
+      <c r="U41" s="8">
+        <v>0.93007</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
+      <c r="A42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="5">
+        <v>10781</v>
+      </c>
+      <c r="C42" s="7">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="D42" s="7">
+        <v>96.5</v>
+      </c>
+      <c r="E42" s="8">
+        <v>0.0026</v>
+      </c>
+      <c r="F42" s="8">
+        <v>0.00715</v>
+      </c>
+      <c r="G42" s="8">
+        <v>0.00631</v>
+      </c>
+      <c r="H42" s="8">
+        <v>0.00659</v>
+      </c>
+      <c r="I42" s="8">
+        <v>0.007979999999999999</v>
+      </c>
+      <c r="J42" s="8">
+        <v>0.01263</v>
+      </c>
+      <c r="K42" s="8">
+        <v>0.01244</v>
+      </c>
+      <c r="L42" s="8">
+        <v>0.01253</v>
+      </c>
+      <c r="M42" s="8">
+        <v>0.01838</v>
+      </c>
+      <c r="N42" s="8">
+        <v>0.02005</v>
+      </c>
+      <c r="O42" s="8">
+        <v>0.02191</v>
+      </c>
+      <c r="P42" s="8">
+        <v>0.02655</v>
+      </c>
+      <c r="Q42" s="8">
+        <v>0.03742</v>
+      </c>
+      <c r="R42" s="8">
+        <v>0.05116</v>
+      </c>
+      <c r="S42" s="8">
+        <v>0.06081</v>
+      </c>
+      <c r="T42" s="8">
+        <v>0.07724</v>
+      </c>
+      <c r="U42" s="8">
+        <v>0.6182299999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
+      <c r="A43" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="5">
+        <v>6153</v>
+      </c>
+      <c r="C43" s="7">
+        <v>100</v>
+      </c>
+      <c r="D43" s="7">
+        <v>88.5</v>
+      </c>
+      <c r="E43" s="8">
+        <v>0.04648</v>
+      </c>
+      <c r="F43" s="8">
+        <v>0.04469</v>
+      </c>
+      <c r="G43" s="8">
+        <v>0.01511</v>
+      </c>
+      <c r="H43" s="8">
+        <v>0.00683</v>
+      </c>
+      <c r="I43" s="8">
+        <v>0.00455</v>
+      </c>
+      <c r="J43" s="8">
+        <v>0.00585</v>
+      </c>
+      <c r="K43" s="8">
+        <v>0.00471</v>
+      </c>
+      <c r="L43" s="8">
+        <v>0.00423</v>
+      </c>
+      <c r="M43" s="8">
+        <v>0.00423</v>
+      </c>
+      <c r="N43" s="8">
+        <v>0.00325</v>
+      </c>
+      <c r="O43" s="8">
+        <v>0.00569</v>
+      </c>
+      <c r="P43" s="8">
+        <v>0.00439</v>
+      </c>
+      <c r="Q43" s="8">
+        <v>0.00796</v>
+      </c>
+      <c r="R43" s="8">
+        <v>0.01089</v>
+      </c>
+      <c r="S43" s="8">
+        <v>0.02064</v>
+      </c>
+      <c r="T43" s="8">
+        <v>0.05282</v>
+      </c>
+      <c r="U43" s="8">
+        <v>0.75768</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
+      <c r="A44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="5">
+        <v>2718</v>
+      </c>
+      <c r="C44" s="7">
+        <v>89.59999999999999</v>
+      </c>
+      <c r="D44" s="7">
+        <v>18.7</v>
+      </c>
+      <c r="E44" s="8">
+        <v>0.62669</v>
+      </c>
+      <c r="F44" s="8">
+        <v>0.09569</v>
+      </c>
+      <c r="G44" s="8">
+        <v>0.05421</v>
+      </c>
+      <c r="H44" s="8">
+        <v>0.03901</v>
+      </c>
+      <c r="I44" s="8">
+        <v>0.01971</v>
+      </c>
+      <c r="J44" s="8">
+        <v>0.01478</v>
+      </c>
+      <c r="K44" s="8">
+        <v>0.00903</v>
+      </c>
+      <c r="L44" s="8">
+        <v>0.0078</v>
+      </c>
+      <c r="M44" s="8">
+        <v>0.00287</v>
+      </c>
+      <c r="N44" s="8">
+        <v>0.00411</v>
+      </c>
+      <c r="O44" s="8">
+        <v>0.00287</v>
+      </c>
+      <c r="P44" s="8">
+        <v>0.00452</v>
+      </c>
+      <c r="Q44" s="8">
+        <v>0.00287</v>
+      </c>
+      <c r="R44" s="8">
+        <v>0.00287</v>
+      </c>
+      <c r="S44" s="8">
+        <v>0.00452</v>
+      </c>
+      <c r="T44" s="8">
+        <v>0.00616</v>
+      </c>
+      <c r="U44" s="8">
+        <v>0.10226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the supplementary figure for the pyDamage results
</commit_message>
<xml_diff>
--- a/06-figures_tables/Dataset_S2.xlsx
+++ b/06-figures_tables/Dataset_S2.xlsx
@@ -7832,7 +7832,7 @@
         <v>100</v>
       </c>
       <c r="D4" s="7">
-        <v>51.5</v>
+        <v>44</v>
       </c>
       <c r="E4" s="8">
         <v>0.17516</v>
@@ -7897,7 +7897,7 @@
         <v>99.59999999999999</v>
       </c>
       <c r="D5" s="7">
-        <v>26.9</v>
+        <v>24</v>
       </c>
       <c r="E5" s="8">
         <v>0.13761</v>
@@ -7962,7 +7962,7 @@
         <v>75</v>
       </c>
       <c r="D6" s="7">
-        <v>99.90000000000001</v>
+        <v>98.8</v>
       </c>
       <c r="E6" s="8">
         <v>4E-05</v>
@@ -8027,7 +8027,7 @@
         <v>27.6</v>
       </c>
       <c r="D7" s="7">
-        <v>99.59999999999999</v>
+        <v>98.09999999999999</v>
       </c>
       <c r="E7" s="8">
         <v>0.0005999999999999999</v>
@@ -8092,7 +8092,7 @@
         <v>96.3</v>
       </c>
       <c r="D8" s="7">
-        <v>77.59999999999999</v>
+        <v>72.90000000000001</v>
       </c>
       <c r="E8" s="8">
         <v>0.07142999999999999</v>
@@ -8157,7 +8157,7 @@
         <v>100</v>
       </c>
       <c r="D9" s="7">
-        <v>100</v>
+        <v>99.40000000000001</v>
       </c>
       <c r="E9" s="8">
         <v>0</v>
@@ -8222,7 +8222,7 @@
         <v>28.5</v>
       </c>
       <c r="D10" s="7">
-        <v>98.90000000000001</v>
+        <v>86.3</v>
       </c>
       <c r="E10" s="8">
         <v>0</v>
@@ -8287,7 +8287,7 @@
         <v>99.90000000000001</v>
       </c>
       <c r="D11" s="7">
-        <v>65.90000000000001</v>
+        <v>60.4</v>
       </c>
       <c r="E11" s="8">
         <v>0.01006</v>
@@ -8352,7 +8352,7 @@
         <v>100</v>
       </c>
       <c r="D12" s="7">
-        <v>90.90000000000001</v>
+        <v>85.3</v>
       </c>
       <c r="E12" s="8">
         <v>0.00032</v>
@@ -8417,7 +8417,7 @@
         <v>99.8</v>
       </c>
       <c r="D13" s="7">
-        <v>92.8</v>
+        <v>87.59999999999999</v>
       </c>
       <c r="E13" s="8">
         <v>0.00614</v>
@@ -8482,7 +8482,7 @@
         <v>99.90000000000001</v>
       </c>
       <c r="D14" s="7">
-        <v>77.90000000000001</v>
+        <v>71.2</v>
       </c>
       <c r="E14" s="8">
         <v>0.00529</v>
@@ -8547,7 +8547,7 @@
         <v>100</v>
       </c>
       <c r="D15" s="7">
-        <v>78.3</v>
+        <v>70.40000000000001</v>
       </c>
       <c r="E15" s="8">
         <v>0.01491</v>
@@ -8612,7 +8612,7 @@
         <v>100</v>
       </c>
       <c r="D16" s="7">
-        <v>21.7</v>
+        <v>16.7</v>
       </c>
       <c r="E16" s="8">
         <v>0.00209</v>
@@ -8677,7 +8677,7 @@
         <v>99.90000000000001</v>
       </c>
       <c r="D17" s="7">
-        <v>99.7</v>
+        <v>90.09999999999999</v>
       </c>
       <c r="E17" s="8">
         <v>0</v>
@@ -8742,7 +8742,7 @@
         <v>99.8</v>
       </c>
       <c r="D18" s="7">
-        <v>31.5</v>
+        <v>25.8</v>
       </c>
       <c r="E18" s="8">
         <v>0.18006</v>
@@ -8807,7 +8807,7 @@
         <v>10.2</v>
       </c>
       <c r="D19" s="7">
-        <v>96.90000000000001</v>
+        <v>90.40000000000001</v>
       </c>
       <c r="E19" s="8">
         <v>0.00021</v>
@@ -8872,7 +8872,7 @@
         <v>100</v>
       </c>
       <c r="D20" s="7">
-        <v>84.2</v>
+        <v>60</v>
       </c>
       <c r="E20" s="8">
         <v>0.00374</v>
@@ -8937,7 +8937,7 @@
         <v>99.90000000000001</v>
       </c>
       <c r="D21" s="7">
-        <v>98</v>
+        <v>86.5</v>
       </c>
       <c r="E21" s="8">
         <v>0.00458</v>
@@ -9002,7 +9002,7 @@
         <v>99.90000000000001</v>
       </c>
       <c r="D22" s="7">
-        <v>73.09999999999999</v>
+        <v>66.5</v>
       </c>
       <c r="E22" s="8">
         <v>0.009560000000000001</v>
@@ -9067,7 +9067,7 @@
         <v>100</v>
       </c>
       <c r="D23" s="7">
-        <v>93.90000000000001</v>
+        <v>91.09999999999999</v>
       </c>
       <c r="E23" s="8">
         <v>0.00484</v>
@@ -9132,7 +9132,7 @@
         <v>100</v>
       </c>
       <c r="D24" s="7">
-        <v>82.90000000000001</v>
+        <v>78</v>
       </c>
       <c r="E24" s="8">
         <v>0.009039999999999999</v>
@@ -9197,7 +9197,7 @@
         <v>99.90000000000001</v>
       </c>
       <c r="D25" s="7">
-        <v>99.59999999999999</v>
+        <v>91</v>
       </c>
       <c r="E25" s="8">
         <v>9.000000000000001E-05</v>
@@ -9262,7 +9262,7 @@
         <v>96</v>
       </c>
       <c r="D26" s="7">
-        <v>58.7</v>
+        <v>49.7</v>
       </c>
       <c r="E26" s="8">
         <v>0.28261</v>
@@ -9327,7 +9327,7 @@
         <v>63.7</v>
       </c>
       <c r="D27" s="7">
-        <v>99.7</v>
+        <v>97.5</v>
       </c>
       <c r="E27" s="8">
         <v>0</v>
@@ -9392,7 +9392,7 @@
         <v>100</v>
       </c>
       <c r="D28" s="7">
-        <v>99.59999999999999</v>
+        <v>95.7</v>
       </c>
       <c r="E28" s="8">
         <v>0.00012</v>
@@ -9457,7 +9457,7 @@
         <v>99.8</v>
       </c>
       <c r="D29" s="7">
-        <v>99.5</v>
+        <v>97.40000000000001</v>
       </c>
       <c r="E29" s="8">
         <v>0.00233</v>
@@ -9522,7 +9522,7 @@
         <v>89.90000000000001</v>
       </c>
       <c r="D30" s="7">
-        <v>98.90000000000001</v>
+        <v>94.90000000000001</v>
       </c>
       <c r="E30" s="8">
         <v>0.00013</v>
@@ -9587,7 +9587,7 @@
         <v>23.4</v>
       </c>
       <c r="D31" s="7">
-        <v>95.3</v>
+        <v>90.59999999999999</v>
       </c>
       <c r="E31" s="8">
         <v>0.00033</v>
@@ -9652,7 +9652,7 @@
         <v>64.90000000000001</v>
       </c>
       <c r="D32" s="7">
-        <v>88.3</v>
+        <v>62</v>
       </c>
       <c r="E32" s="8">
         <v>0.01291</v>
@@ -9717,7 +9717,7 @@
         <v>37.3</v>
       </c>
       <c r="D33" s="7">
-        <v>94.8</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="E33" s="8">
         <v>0.00076</v>
@@ -9782,7 +9782,7 @@
         <v>99.40000000000001</v>
       </c>
       <c r="D34" s="7">
-        <v>52.8</v>
+        <v>48.6</v>
       </c>
       <c r="E34" s="8">
         <v>0.11811</v>
@@ -9847,7 +9847,7 @@
         <v>100</v>
       </c>
       <c r="D35" s="7">
-        <v>99.09999999999999</v>
+        <v>95.40000000000001</v>
       </c>
       <c r="E35" s="8">
         <v>6.999999999999999E-05</v>
@@ -9912,7 +9912,7 @@
         <v>99.90000000000001</v>
       </c>
       <c r="D36" s="7">
-        <v>93.8</v>
+        <v>88.3</v>
       </c>
       <c r="E36" s="8">
         <v>0.00143</v>
@@ -9977,7 +9977,7 @@
         <v>99.90000000000001</v>
       </c>
       <c r="D37" s="7">
-        <v>95.3</v>
+        <v>88.2</v>
       </c>
       <c r="E37" s="8">
         <v>0.00135</v>
@@ -10042,7 +10042,7 @@
         <v>99.90000000000001</v>
       </c>
       <c r="D38" s="7">
-        <v>92.8</v>
+        <v>86.7</v>
       </c>
       <c r="E38" s="8">
         <v>0.00135</v>
@@ -10107,7 +10107,7 @@
         <v>82.8</v>
       </c>
       <c r="D39" s="7">
-        <v>98.5</v>
+        <v>89.40000000000001</v>
       </c>
       <c r="E39" s="8">
         <v>0.00044</v>
@@ -10172,7 +10172,7 @@
         <v>65.7</v>
       </c>
       <c r="D40" s="7">
-        <v>99.7</v>
+        <v>91.8</v>
       </c>
       <c r="E40" s="8">
         <v>5E-05</v>
@@ -10237,7 +10237,7 @@
         <v>100</v>
       </c>
       <c r="D41" s="7">
-        <v>95</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="E41" s="8">
         <v>0.0035</v>
@@ -10302,7 +10302,7 @@
         <v>99.90000000000001</v>
       </c>
       <c r="D42" s="7">
-        <v>96.5</v>
+        <v>85.90000000000001</v>
       </c>
       <c r="E42" s="8">
         <v>0.0026</v>
@@ -10367,7 +10367,7 @@
         <v>100</v>
       </c>
       <c r="D43" s="7">
-        <v>88.5</v>
+        <v>73</v>
       </c>
       <c r="E43" s="8">
         <v>0.04648</v>
@@ -10432,7 +10432,7 @@
         <v>89.59999999999999</v>
       </c>
       <c r="D44" s="7">
-        <v>18.7</v>
+        <v>15.2</v>
       </c>
       <c r="E44" s="8">
         <v>0.62669</v>

</xml_diff>